<commit_message>
Get daily reddit data: Tue May 20 08:13:02 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_05_25.xlsx
+++ b/data/collected_data/2025_05_25.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C480"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3049 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1kqz9ws</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>All the quotes I thought about were cringe.</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5xjqgub47w1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1kqz1n1</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Lava Nails</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqz1n1</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1kqy5p3</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Attaching full cover gel extensions</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kqy5p3/attaching_full_cover_gel_extensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1kqxu9o</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Just wanted to show off nails I decided to get done!</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqxu9o</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1kqwoqm</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Under the sea 🐙🪼🐚⭐️🪸</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqwoqm</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1kqx1a5</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Y’all think these look ok?</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqx1a5</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1kqwxg1</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>What shape would suit me best?</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ebajv8d6ev1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1kqwwmx</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Showing off nail growth progress</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqwwmx</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1kqwslt</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Nailtiques Formula 2 Plus in Canada?</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kqwslt/nailtiques_formula_2_plus_in_canada/</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1kqwsl9</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>my mermaid nails!!</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqwsl9</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1kqwl2o</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Gel x vs acrylic/hard gel nails wedding nails</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kqwl2o/gel_x_vs_acrylichard_gel_nails_wedding_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1kqwh93</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Looking for a polish in this shade :-)</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/upkyinka9v1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1kque4e</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Chromed them myself…</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kque4e</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1kqw0lh</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Biogel 48$</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqw0lh</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1kqw05j</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Thoughts on red carpet gel?</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kqw05j/thoughts_on_red_carpet_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1kqvzhr</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Help , i wanna improve how my nails look</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqvzhr</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1kqvj07</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Sally Hansen Vit E Nail Oil Still Okay After Years of Not Being Used</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kqvj07/sally_hansen_vit_e_nail_oil_still_okay_after/</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1kqve18</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>This pink design is the one I'm most happy with.</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p0wd0rzzxu1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1kqvdcp</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Got Taurus ♉️  themed nails for my birthday</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqvdcp</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1kqva5d</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Suggestions?</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqva5d</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1kquh1p</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Is This Fungi?</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kquh1p</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1kqu358</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Orly breathable nail polish</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqu358</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1kqtszk</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Undersea/mermaid vibes</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yzcxxrk1ju1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1kqtm6e</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Magic Card Monday</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqtm6e</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1kqtdpb</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Was in the mood for something fun</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qarm50l8fu1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1kqt7c2</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Candy Nails I Did Today</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d7lnca4mdu1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1kqt53p</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Should I redo my nails? Tried a new shape and color. My right hand looks really lumpy 😩 (builder gel)</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqt53p</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1kqt3q5</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Autumnal/winter nails 🐞</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqt3q5</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1kqt24p</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Sort of Early Summer nails</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j75n20zbcu1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1kqsv5j</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>This shade of pink is one of my favorites for my nails.</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3or6yw9kau1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1kqsfkk</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>My favorite set I've made so far 💜</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/do3edqno6u1f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1kqqyed</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Still obsessed with chrome..</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqqyed</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1kqs9rw</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Newest set</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqs9rw</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1kqnyez</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Nail tech eats again 🤧</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5rm0lp6a5t1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1kqs2he</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Some of the mani/pedis I’ve had over the years</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqs2he</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1kqs0cr</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>I just add my fav nails I do last year</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqs0cr</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1kqs0b9</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Obsessed with my newest set! Gothic moody vibes 🖤🤍</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqs0b9</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1kqry4c</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Natural nails</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqry4c</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1kqrxnc</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Just been playing around with a few press on sets of my own 🩷 beginner girly who loves lil charms</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqrxnc</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1kqrtw2</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>HOPE Y’ALL HAD A GOOD MONDAY, it’s hard out here</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ou5dc0s71u1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1kqrp53</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Between being tiny and constant biting, I really dislike my nails</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqrp53</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1kqrhbj</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Every time🥴</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7r8msnb2yt1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1kqrdqq</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Are my nails ok?</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/63fe5dt5xt1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1kqrche</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Nail adhesive tabs?</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gaq3s30vwt1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1kqr4ii</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Alice in wonderland nails</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqr4ii</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1kqqeus</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Third acrylic set ever!</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/axtso7oqot1f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1kqqd14</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Finally, nails that ask "would you love me if I was a worm?"</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqqd14</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1kqpvkr</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>How to handle walk ins and appointments better as a new receptionist</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kqpvkr/how_to_handle_walk_ins_and_appointments_better_as/</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1kqpjpl</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Need help!</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kqpjpl/need_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1kqp4vx</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>New favorite press on nail brand and color🥰</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqp4vx</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1kqov21</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Hermosas verdad?</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/atv241n3ct1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1kqooal</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>My nail tech thinks I’m boring?</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kqooal/my_nail_tech_thinks_im_boring/</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1kqo9iq</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Fave set ever</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqo9iq</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1kqnllc</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Discoloration?!?!?</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/du2d0pkq2t1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1kqnwdm</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>What shape would suit my hands best?</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qoh65yqv4t1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1kqndys</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>First time making my own press ons</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqndys</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1kqmzpe</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Fresh nails!</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqmzpe</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1kqmwm0</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>An previous set</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3zdfykjqxs1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1kql8uy</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>RIP (not literally)</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kql8uy</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1kqm4c1</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Love My Aura Nail😍</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nhgqz5a9ss1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1kqm3t7</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Just sharing my birthday nails</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqm3t7</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1kqlz3m</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Free Hand French Tips</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xwpg2wx8rs1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1kqly6s</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>new set i did #love this typa pose for showing of my nails</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqly6s</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1kqlvyf</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>New Dazzle Dry mani💜</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqlvyf</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1kqlmww</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>My nails haven’t grown out in a week</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqlmww</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1kqlmmt</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>I love this color!! 🥰🥰</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yzq0dgiros1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1kqlgbz</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Birthday nails!!</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m1x26jelns1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1kqey2l</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>How do I heal the calloused skin around my nails??</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ag0ugxneer1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1kqjhze</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Cats Eye, Oh My.</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rbx28962as1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1kqkbr9</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Luxury nail charms? Where do I find them?</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kqkbr9/luxury_nail_charms_where_do_i_find_them/</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1kqk4p7</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Went to a pretty new nail tech, am in love with my set!</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqk4p7</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1kqk3me</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>First time doing gel nails at home 💕</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0lwvt285es1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1kqjihc</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Tulips 🌷</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqjihc</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1kqj8ca</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>how do they look?🌸</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xdgi8ka78s1f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1kpyf5a</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>What brand is this?</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cm0pa5aesm1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1kqimnq</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>just got a mani/pedi… what do you think?</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqimnq</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1kqilkq</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>First time getting gel-x extensions</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqilkq</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1kqidfa</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Builder gel with a tech, always lifts 🙃</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqidfa</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1kqibwq</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>What nail shape would suit me best?</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/13cq8gx02s1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1kqgdkv</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Safe UV cure nail glue for at home nails?</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kqgdkv/safe_uv_cure_nail_glue_for_at_home_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1kqhtls</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>I love my Ditto nails :3</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqhtls</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1kqhsmh</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Feedback wanted, does this nude color fit me?</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqhsmh</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1kqhfhh</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Tried a little bit of nail art</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqhfhh</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1kqhcd2</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>did these for the beach. cant tell if i love them or hate them please give me your opinions. dont worry im gonna shave my toes 🙈</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2plg3n98vr1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1kqh6h4</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>My little brother did my nails. Did he cook chat?</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqh6h4</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1kqh460</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Tried a deeper green and more squared</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/smok25intr1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1kqgl5w</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Linda give me a manicure?</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ix3qd162qr1f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1kqgjgr</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>what do u call this</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqgjgr</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1kqgcch</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Obsessed! Just got nails again after years without them</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d2axchhaor1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1kqg7wb</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>new favorite color combo 🐍🌿🦎</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqg7wb</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1kqfxe1</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Learning to do my own poly gel nails</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqfxe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1kqfwdk</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Best practice for this break?</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fj3y48k7lr1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1kqfl9t</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>new 💅💅💅💅</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u96lfro0jr1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1kqf7xv</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Broken (big) toenail - advice so my feet can look normal in sandals this summer</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kqf7xv/broken_big_toenail_advice_so_my_feet_can_look/</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1kqf4mz</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Bit grown out but is this a good shape for my hands?</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bdr9g9fpfr1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1kqf1jr</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Learning to do my own nails.</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fqh2g204fr1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1kqev1d</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>My new nail set inspired by Naruto. Let me know what you think! 👁️⚔️🌪️</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqev1d</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1kqen5n</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>My friend made me some beautiful Expedition 33 themed nails 😍</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/apojxbc8cr1f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1kqeld6</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>5 Months Down the Drain 😭 RIP to My Favorite Nail</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7uqz6xmvbr1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1kqed64</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Nails I got done yesterday!</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqed64</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1kqzdd7</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Finally Swatched My Collection, Now To Figure Out How To Sort Them In Rainbow Order!</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqzdd7</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1kqy7h0</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Started doing nails here’s a few sets I’ve done</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqy7h0</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1kqwdkk</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Finally cabochon'd all my 128 polishes. I love it.</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqwdkk</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1kqvomp</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Neon!! Ready for summer 🌞</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqvomp</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1kqvmso</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>What is the best drying drops ?</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kqvmso/what_is_the_best_drying_drops/</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1kqvizl</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Attempted to dupe the May PPU shade Toucan Play that Game by Pinnacle Polish, how did I do?</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqvizl</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1kqvftw</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Do all jellies take forever to dry? Or only Cirque?</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r6yvdtfnyu1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1kquf1p</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Topper stuff</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kquf1p/topper_stuff/</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1kquazs</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Took a picture of my cat and instead shocked my non polish friends.</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v98p893mnu1f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1kqtmu8</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Magic Card Monday</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqtmu8</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1kqt1d9</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Randomly grabbed an old PPU polish and was pleasantly surprised!</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqt1d9</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1kqsy91</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Can I put a press on over this?</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/axuzby3dbu1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1kqsabe</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Thought you wonderful people would appreciate my spread here</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tm3wpknd5u1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1kqs6bl</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Mmm… how do I feel about this one?!</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqs6bl</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1kqqx91</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>First attempt at stain glass nails</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqqx91</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1kqq1lv</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Pearl Treasure Moonstone ⚪🔷</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqpz4o</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1kqp1du</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Future Sight 🌀</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqp1du</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1kqocef</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer haul from the last shop open!</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zshhlax68t1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1kqo0qa</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Swatch Display!</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqo0qa</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1kqnqb2</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Dollar General polish Mani</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqnqb2</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1kqnlnl</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Teeth nails because why not 🤪</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqnlnl</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1kqmlqh</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Glossy Taco is a game changer!</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqmlqh</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1kqmahx</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Nail shaping question</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqmahx</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1kqm05g</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Thanks to this subreddit i finally managed to to the velvet effect!</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bmcumnvfrs1f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1kqlkr5</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Cirque Colors Lolly Jelly</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqlkr5</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1kqkxwx</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Swatch p0rn</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqkxwx</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1kqkrah</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>If you (like me) enjoy watching TV shows or movies while doing your nails, try using the Audio Description!</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kqkrah/if_you_like_me_enjoy_watching_tv_shows_or_movies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1kqkp7j</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Summertime Layering ☀️</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fcjg74wuhs1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1kqk65q</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>[maker pr] New Brand: Vacance</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kqk65q/maker_pr_new_brand_vacance/</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1kqk1nr</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Would you still use this?</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqk1nr</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1kqimqm</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>maelstrom of all evil</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqimqm</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1kqi7cf</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Eerie Silence from Cadillacquer</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eg0kflw51s1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1kqhjjn</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>First attempt at nail art</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqhjjn</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1kqh3xo</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Opinion about the color please ! Ignore the messy application 😔</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqh3xo</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1kqgqtr</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>love this dollar store polish! 🍒</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqgqtr</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1kqgaup</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Whiskey Sunrise🌅</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqgaup</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1kqg5xi</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Favorite rose gold combo ✨💕</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqg5xi</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1kqfstq</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>I'm so happy with this Nail Art 😍</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqfqd5</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1kqeqn0</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Do ya think HR would invite me for a chat if I started a salon in my cubicle?</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kqeqn0/do_ya_think_hr_would_invite_me_for_a_chat_if_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1kqec49</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>enemies to lovers: my favorite book trope!</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/an8ijbtt9r1f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1kqeaaa</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>What's your funniest color fail?</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqeaaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1kqe443</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>i always forget how pretty this shade is. lynb’s cats paw 🐾</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqe443</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1kqdwdb</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Big Reef Energy mani</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqdwdb</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1kqdw7c</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>How can I prevent these hard cracks that form to the side of my nails?</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqdw7c</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1kqdina</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Does anyone know 9ml nail polish it’s gonna be enough?</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kqdina/does_anyone_know_9ml_nail_polish_its_gonna_be/</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1kqcun5</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Can nails be too bendy?</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kqcun5/can_nails_be_too_bendy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1kqcqji</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>My new pastels from Atomic (plus 1 Color Club)</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w03mw2d7xq1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1kqcm0m</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>First Lurid order!</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqcm0m</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1kqclky</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Any chance By Dany Vianna is going to bring back Rosewater for PPU rewind? 🥺</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kqclky/any_chance_by_dany_vianna_is_going_to_bring_back/</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1kqce4j</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Some commotion for the nails?</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqce4j</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1kqc58f</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Clionadh Norpscilosin and Psilocin</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7r13kawvtq1f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1kqbtqv</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Can press ons cause allergies?</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kqbtqv/can_press_ons_cause_allergies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1kqayr4</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Octopus nails</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqayr4</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1kpz44s</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>natural nail growth</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kpz44s/natural_nail_growth/</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1kq1cv7</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>First post: rediscovering nail art!</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kq1cv7</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1kq7x0e</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kq7x0e/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1kqzfah</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Painted myself some Ice cream nails.</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eon9ta419w1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1kqyqe6</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Birthday nails</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vyaqdmi30w1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1kqvk1i</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>A vtuber commission I just finished</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqvk1i</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1kqudfg</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>nail stickers</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kqudfg/nail_stickers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1kqtwwq</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Planning my next set</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hgejtfb0ku1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1kqtiq8</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Spring 🌸</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqtiq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1kqszgo</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>How to improve at hand painting French tips?</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kqszgo/how_to_improve_at_hand_painting_french_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1kqsvnh</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Beginner starting a press on business and hoping for feedback</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqsvnh</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1kqptk3</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>ladybugs🥰</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sajeot9ujt1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1kqnuxi</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>First set I’m actually proud of</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqnuxi</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1kqni5i</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Press on sets from today :)</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqni5i</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1kqmsle</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Cat Eye Attempt #2</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a6foh08yws1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1kqm24g</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>I gifted my niece nail art tool kit for her birthday, and she surprised me</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqm24g</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1kqm0j7</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Ocean theme</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/teiqawrirs1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1kqk417</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>I can’t take picture but whatever there cute anyway, I just wish I was better at line art</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqk417</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1kqk0mk</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Extreme nails, this nail model is the design practice</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hq24ntslds1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1kqhen1</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Is this a bad liner brush?</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/36ohzyvnvr1f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1kqh6ix</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Grungy and glitter</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ua395sp3ur1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1kqf54c</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>First time doing French tips. Advice?</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqf54c</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1kqd5ii</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Clown nails!</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e7u3brhg1r1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1kqbsd1</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Currently planning my next nail design- which chrome fits the best?</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqbsd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1kqamcg</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Flowers 🤍🖤</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kqamcg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1kq826m</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Enjoy your bananas🍌😍💅🏻</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kq826m</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed May 21 08:12:35 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_05_25.xlsx
+++ b/data/collected_data/2025_05_25.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C480"/>
+  <dimension ref="A1:C663"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8593,6 +8593,3117 @@
         </is>
       </c>
     </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1krrf3x</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Using builder gel with polygel?</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1krrf3x/using_builder_gel_with_polygel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1krrdv1</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>3rd time I did my own nails, so proud of them!!</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krrdv1</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1krqxpm</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Juicy tropical animal print Press Ons I made</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/abzj24afv22f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1krqq3g</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>My beautiful creation very striking</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4fdr9400t22f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1krqci9</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Moo deng nails</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krqci9</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1krqaxl</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Just wanted to show off my girlfriends nails. She did them herself.</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/reky9h94o22f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1krozb9</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Is nylon fiber good for your nails?</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1krozb9/is_nylon_fiber_good_for_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1kro813</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>SNS dip powder with chrome</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wrqis5nw122f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1krmk53</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Need help picking my next set, I wanted to redo an old set, can you guys help me pick?!</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krmk53</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1krnb6d</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Girlfriend needs help!</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krnb6d</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1krnu7g</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Some of the mani/pedis I’ve had over the years (Pt. 2)</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krnu7g</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1krksbo</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Fix a break on natural nails with gel strip</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krksbo</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1krnnqt</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>My god I love chrome</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krnnqt</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1krn9ya</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Will my nails match my prom  dress?</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krn9ya</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1krmu1c</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Summer Nails</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0il8qhiso12f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1krmku7</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>I did my bff's nails after a break up, freaking love the new gelx tips I got just for her, what do you think?</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krmku7</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1krmfq2</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>My coworker let me do her birthday nails!</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nhryxyy5l12f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1krmfig</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Our Kid Loves Doing Nails</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1zsh51o2l12f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1krmeuo</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>This is so mesmerising</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i5686q5xk12f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1krmcj9</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Hello, I need advice in how to start doing nails, I want to take a course in my country but I want to excel in it, in my country there is a few great nail artists, there is more regular ones. I would like to know the list of materials and tools I need to do great nails as the ones in the picture.</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ss2outfbk12f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1krlpf9</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Calico Critter Nails</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krlpf9</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1krlnkb</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>How To Find a Tech</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1krlnkb/how_to_find_a_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1krlhw0</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>It’s citrus season 🍊💅</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ympoafqic12f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1krl5ur</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>flowers for the summer 🌻💕</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krl5ur</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1krl6lw</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>so proud of my natural nails ❤️</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krl6lw</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1krknc6</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>My Graduation Nails 🎓</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krknc6</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1kreuai</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>BIAB growth pain??</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kreuai/biab_growth_pain/</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1krinpz</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Nail damage from gripping my desk</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krinpz</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1krirso</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Pinterest inspired nails!</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fvh693nqo02f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1krjgpc</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Sorry for the long post, need your opinions. My nail girl is visiting family in China so I saw someone else… it was a disaster😩</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krjgpc</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1krjqm3</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Looking for a specific nail color</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krjqm3</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1krjor0</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Cowboy Carter Nails</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krjor0</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1krjmp8</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Satin + Flowers</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krjmp8</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1kris0u</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Pink aura with chrome 😍🩷</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kris0u</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1krio7a</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>First time</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krio7a</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1krinid</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Acrylic press ons or no acrylic on the press ons</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1krinid/acrylic_press_ons_or_no_acrylic_on_the_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1krhvmf</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>My Mofusand Strawberry Nails 🍓🐱🎀</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krhvmf</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1krhttp</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Summer neons</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krhttp</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1krhnmp</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>cowboy carter nail set</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krhnmp</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1krhhll</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Finally able to grow my natural nails</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krhhll</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1krhhb4</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Builder Gel!</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krhhb4</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1krhh16</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Long pinkies</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j578ub6fe02f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1krduq1</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>First time acrylics and my nails are ruined</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krduq1</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1krg7zz</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>How do you measure nail size??</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krg7zz</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1krg6au</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>My first acrylics (male)</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krg6au</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1krfv6k</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Non gel cat-eye / magnetic manicure?</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1krfv6k/non_gel_cateye_magnetic_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1krfs7m</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Thoughts?</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qdf6zthp102f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1krfc2v</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>not feeling this set</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/52pg5zggyz1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1krf9pr</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Are acrylic nails good for growing nails out?</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1krf9pr/are_acrylic_nails_good_for_growing_nails_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1krf19b</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Is Mooncat Polish worth the price tag?</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1krf19b/is_mooncat_polish_worth_the_price_tag/</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1krewex</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>First time with a flower 🌼</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krewex</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1krevkk</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Love a good pinkkkkk</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5sri8z54vz1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1krekq9</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Went for a shimmery pink</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0zt7g3vwsz1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1krdjpm</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>What happened here</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krdjpm</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1kre5z9</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Lemon blueberry 🫐 🍋</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kre5z9</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1kre572</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Red nails</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/47koyuctpz1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1kre39y</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Guy I met on bumble did my nails for me!!</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kre39y</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1krdxe0</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>First time trying nail art!</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/puaer0d9oz1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1krdr98</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>♥️queen of hearts♥️ nails</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krdr98</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1krdmw1</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Green cat eye and gold</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krdmw1</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1krdiyc</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Ice Cream nails</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j40xvpbdlz1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1krdbrl</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Pastel ombré swirls💕</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krdbrl</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1krd95e</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Me and my short nails can finally participate.</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zcpmhfzejz1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1krcgdb</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>One of my favorite designs I ever got! 🩵</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/axsbrx1pdz1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1krc3kp</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Got my nails done for Prom</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krc3kp</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1krbwjr</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>One of my favorite sets!🍒❤️🍒🎀🍒💋🍒</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krbwjr</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1krbu2b</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>So in love with these</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krbu2b</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1krbtp6</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>🧼🫧☁️ what is the best chrome powder brand? ☁️🫧🧼</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c6ym7md99z1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1krbpbn</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Don't worry, be cappy</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krbpbn</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1krbgxt</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>I keep it juicy juicy</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krbgxt</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1kran4b</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Striped French</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uweiqsh41z1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1kragv9</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>The perfect pink</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kragv9</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1kr9t29</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Anyone with no pinky toe nails know a way to fake one?</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kr9t29/anyone_with_no_pinky_toe_nails_know_a_way_to_fake/</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1kr9ddj</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Got my nails done for prom.</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kr9ddj</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1kr99bh</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>First ever nail art on myself!</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/leuctdngry1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1kr94l7</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>I’m in love</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2xs7kb5jqy1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1kr91gv</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>this weeks set</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kr91gv</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1kr8y67</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Recovering from a rough patch</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kr8y67</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1kr8um4</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Thin nails and Semi cured gel nail strips</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kr8um4/thin_nails_and_semi_cured_gel_nail_strips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1kr8rq1</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>First time gel tips, art, everything! So proud :)</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kr8rq1</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1kr8g08</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Do we like?</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kr8g08</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1kr888u</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>My first nails!</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kgc31cm6ky1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1kqsdzu</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Can I put press ons over this?</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jpgz7o6a6u1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1kr1mno</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Havent gotten my nails done in years (plus a collagen disorder)</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kr1mno/havent_gotten_my_nails_done_in_years_plus_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1kr5zpb</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Advice on how to glue tips</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kr5zpb/advice_on_how_to_glue_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1kr667k</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Looking for dupes of this lovely Barry M polish!</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kr667k</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1kr6b7v</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>New favourite combination</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kr6b7v</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1kr6xmn</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Looking for a dupe of smores than a feeling from Colores de Carol</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/revftn1yay1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1kr7veg</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Made by me💅🏻</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kr7veg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1kr7tqa</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Are metal nail files so terrible that they never get mentioned? (AKA, why do I only see emery boards/glass nail files?)</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kr7tqa/are_metal_nail_files_so_terrible_that_they_never/</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1kr7stz</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>First attempt at French tips :)</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hdyjuu44hy1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1kr7ll4</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Spring/Summer Nails</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kr7ll4</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1kr7h8w</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>If you give a mouse a strawberry 🍓</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3p1lde2uey1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1kr7f3b</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Next set</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x63i7z8eey1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1kr7er2</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Obsessed with matte black!</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kr7er2</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1kr78xp</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Two different colours on each hand</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kr78xp</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1kr74k5</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Mooncat magnetic nail polish</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kr74k5</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1kr4jdj</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>These press ons have been on for over a week, survived 1.5 hours in the pool and the sauna! - With sticky tabs!</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/waf9tl25sx1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1kr2v71</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>How do you make press ons like these? Image credit: @chlawed on Instagram</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kr2v71</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1kr6qjb</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Matte Top Coat</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kr6qjb/matte_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1krr4ho</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Warm Skittle</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krr4ho</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1krq07t</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>First time wearing purple in a long time and I'm in love 💜</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krq07t</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1krpijj</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>First Time Water Marble</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xjaiz5sef22f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1krnsa2</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Alchemy Lacquers - Snuggie Huggie</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dr5wz5cpx12f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1krmpty</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>How to regrow nail bed?</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1krmpty/how_to_regrow_nail_bed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1krlr5y</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Getting into nail art. Any tips?</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1krlr5y/getting_into_nail_art_any_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1krlmqj</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Fairycore 🧚‍♂️🦋🍀</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/33laydcrd12f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1krl5te</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Linear brown holo death match</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krl5te</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1krl1zf</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Why peeling?</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/niwnnwmd812f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1krkrg5</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Favorite reflective polishes?</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1krkrg5/favorite_reflective_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1krkcym</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Looking for a dupe of the LE Sinful Colors x Kylie "Holly-Wood"</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hjzd8lu7212f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1krkar1</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Silk wrap question</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1krkar1/silk_wrap_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1krk1xz</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Having fun with layering!</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uwf04zg1z02f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1krjfhv</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Feeling Springy💚🧡</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krjfhv</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1kri3wc</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>The Dark Urge just changed my life</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kri3wc</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1kri3us</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Gel dupe for mooncat midnight drive?</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kri3us</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1kri3qh</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Here's my claw haul! Which one should I sport next? Decisions, decisions. 😅😍✨️💕💖</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mmsfi6qbj02f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1krhfp1</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>No amount of prep stops the peeling</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1krhfp1/no_amount_of_prep_stops_the_peeling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1krgwei</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Bad gel manicure - had to fix at home to</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krgwei</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1krgt09</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>5 free vs 7 free vs 10 free</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1krgt09/5_free_vs_7_free_vs_10_free/</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1krg1q6</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Birthday Nails and a book I finished.</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krg1q6</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1krfbih</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>First ILNP order — what should I be buying???</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1krfbih/first_ilnp_order_what_should_i_be_buying/</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1krfb79</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Help match my nails to this car</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krfb79</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1krf11a</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>You gotta go BLAP</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0k7groj6vz1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1kreupj</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Short nail inspo</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kreupj/short_nail_inspo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1krejxw</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Putting off chopping the vamp fangs down</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krejxw</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1kr9948</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Beginner trying soft gel nails</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kr9948</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1krbxvi</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Showing off My New Glitter Teal Nails !</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krbxvi</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1krecqd</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Dupe for this barbie pink</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oz6r6z2crz1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1kre9m5</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>One coat of Fata Morgana</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kre9m5</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1kre5xe</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>I jumped on the cabochon train and hopped off at the jewelry stop!</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kre5xe</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1kre1pn</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>And they all looked so pretty :(</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gu1o5df4pz1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1krdk0j</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>"I’m Not Really A Waitress" but in emerald green?</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1krdk0j/im_not_really_a_waitress_but_in_emerald_green/</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1krdgfe</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Mist Over the Thames in the bathroom light (plus bonus daylight shots)</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krdgfe</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1krd5ki</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>ILNP pinks for neutral skin tones</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1krd5ki/ilnp_pinks_for_neutral_skin_tones/</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1krcszs</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Nail polish chipping on the side of my nail?</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sx7s3q78gz1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1krcrg9</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Randomly picked mani 🧡💜</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krcrg9</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1krci2f</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>My boss got me Mooncat as a “just because” gift 😭</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krci2f</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1krcexm</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>After the Rain is such a fitting name for this shade ☔️</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krcexm</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1krbwm3</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>"Mojito" making me feel better about a gray PNW spring day 🍹</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l14mn13u9z1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1krbqga</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>A Very Rough French Mani</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krbqga</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1krawv5</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Fail but also I kind of like this</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krawv5</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1krau7h</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Getting super antsy for summer neons, but whyy does the black light have to illuminate application oopsies</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krau7h</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1kr9zsg</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>I want to cry</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7v5qlkemwy1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1kr9szu</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Okay Bog Dweller!</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6t8hzel8vy1f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1kr9oer</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>rainbow eucalyptus by clionadh cosmetics</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kr9oer</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1kr9h72</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Do you ever add nail polish thinner to brand new polish for cleaner applications? Or do I just need to keep working on technique?</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kr9h72</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1kr8nek</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>✨Fancy Fingers✨ GUERLAIN</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gqwevqf5ny1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1kr8gxb</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>I have a silly request - does anyone know a color that looks like Essie Ripple Reflect WITH FLASH?</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kr8gxb</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1kr6yst</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Looking for a dupe of S’mores than a feeling from Colores de Carol</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3qvmzex6by1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1kr602h</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Looking for dupes of this lovely Barry M polish!</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kr602h</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1kr5soj</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>I can never just leave my manicure alone</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kr5soj</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1kr5s5g</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>did you learn something about lacquer/nail care that changed how you view it?</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kr5s5g/did_you_learn_something_about_lacquernail_care/</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1kr3y1q</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Can anyone colour match this lip oil? Preferably a jelly/sheer polish, thanks! (UK)</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kr3y1q</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1kr3kau</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>So juicy I just wanna eat it lol</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kr3kau</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1kr2axe</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>First orange set in ages!</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kr2axe</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1kr1101</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Nail polish chit chat!</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kr1101/nail_polish_chit_chat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1kr00y4</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Some of my collection</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0mriplwzgw1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1kq9zm1</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Are there general “ rules” on what nail shape will suit who?</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kq9zm1/are_there_general_rules_on_what_nail_shape_will/</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1kqlcaf</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Do these look normal?</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3eq2odqsms1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1kqop5g</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Van Gogh inspired nail polish</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3byyr32vat1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1krrg83</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Not my work</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fcif7861232f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1krq5py</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>My juicy tropical press on nail set!</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z87n50jbm22f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1krojbo</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Cool ❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wldsd3n4522f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1krns0n</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>My favourite 🥰</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1hbu2zbnx12f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1krn01v</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Welcome summer 🍋🍋‍🟩</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krn01v</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1krlhpk</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Some nail art on my sister ☺️</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uyq00g7hc12f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1krkpk2</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>My Nails for the Indy 500 this weekend</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krkpk2</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1krjm05</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>I think there's something I'm doing wrong, I ran the magnet through the cat eye, but I think the effect didn't turn out well</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krjm05</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1krjhnn</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Summer Mix and Match Nails</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krjhnn</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1krib7q</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>I’m a rookie</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rl9yuf8zk02f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1krhxpp</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>My Mofusand Strawberry Nails 🍓🐱🎀</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krhxpp</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1krg5u3</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Junk Hawk nails</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krg5u3</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1krf5fn</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>inspo from pinterest</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hrxjczt3xz1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1krethr</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Trying marble effect</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/co8urn8puz1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1krdjx5</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Ice Cream nails</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ijqsk6cklz1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1krbqwk</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Under the Sea 🐙🪼🐚⭐️🪸</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krbqwk</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1krblbi</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Don't worry, be cappy</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krblbi</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1kragqe</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>My favorite Mani (using regular nail polish)</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3idtuqtvzy1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1kr296v</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Cyberpunk inspired set for a trip</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dyimc28b7x1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1kr10lb</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Just a guy that likes mag gels</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kr10lb</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1kr0pc6</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Summer time,sweet memory😍🌸</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kr0pc6</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1kqxjmj</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Acrylic Nail Charms</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kqxjmj/acrylic_nail_charms/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu May 22 08:12:38 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_05_25.xlsx
+++ b/data/collected_data/2025_05_25.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C663"/>
+  <dimension ref="A1:C843"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11704,6 +11704,3066 @@
         </is>
       </c>
     </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1kskwo0</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>My cute short nails</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0mvo9d3dea2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1kskrh2</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>first 🕷️ nails</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ncrmv67hca2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1ksiuzi</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Started Cuticle Oiling!</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/879lwl7gp92f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1ksi5uc</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>How galactic do they look😍</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/325j747nh92f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1kshhxx</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>first set of press ons!</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kshhxx</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1kshcke</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>DIY acrylic manicure</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kshcke</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1ksfih4</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>I’m absolutely obsessed 😭🎀</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/60v19qrjr82f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1ksgj4s</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>nail growth after 3 months!</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksgj4s</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1ksgopa</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Little pink mushrooms for my birthday weekend! Yes, I did them myself</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksgopa</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1ksglxa</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>first time using polygel!</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksglxa</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1ksgbxp</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Been practicing</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mq9rnuvcz82f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1ksfuba</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>The best set by far 💜</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mgrlquymu82f1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1ksfr23</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Pedi done for summer</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b4d1nhcst82f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1ksexvb</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Had a fun idea for an aquarium nail inspired by Junji Ito and painted a lil set 🥰</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/con51x5am82f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1ksf5gm</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>What would you call this shape?</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksf5gm</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1kseph0</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>set for a wedding!</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jtuph8e3k82f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1ksehuj</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>I finally broke free from cat eye…to chrome lol</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksehuj</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1ksegc6</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>does anybody know what this is?</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xyff9n4rh82f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1ksees1</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>My friend has really gotten into gel nails these past few months. I want to get her a birthday gift related to this but I know nothing about this topic. Any gift suggestions? (I'm in Canada- would like to avoid paying customs). She mentioned something about Korean jelly nails too? What's that mean?</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ksees1/my_friend_has_really_gotten_into_gel_nails_these/</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1ksbhyq</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>inspo question!</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cehpum1xr72f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1ksdzzc</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>What would you call this design?</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/25y2ri8jd82f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1ksdr76</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Celestial nails for my birthday!</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksdr76</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1kscsrc</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>My girl did an amazing job with the mouth</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kscsrc</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1ksdafi</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Acrylic</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ksdafi/acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1ksd22e</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>This is one of my favorite nudes.</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zqb6a2q2582f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1kscoel</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Checkered cherries 🍒</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4pihoylu182f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1ksc7v2</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Mooncat nail polish dupes</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/59ashsqwx72f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1ksbuu7</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>first time trying acrylic overlay</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ok8cifwuu72f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1ksbphk</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>hacks for keeping nails clean?</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ksbphk/hacks_for_keeping_nails_clean/</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1ksbh2h</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>New nail day is the best day</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/olx61y4pr72f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1ksb38p</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Beginner Press On Artist</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksb38p</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1ksahtw</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>New nails. HIDE THE BALLOONS 😝</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6obm6tstj72f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1ksac0j</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>my nails need a change 😭</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2hhzi00mi72f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1ks9hpx</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>My pinky nail doesn’t grow round. Anyone else have this?</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3dmltoybc72f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1ks9cq1</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Comfort zone nail polish</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks9cq1</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1ks95c4</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>nails before or after shower</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ks95c4/nails_before_or_after_shower/</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1ks8scd</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Guess how much this costed?</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks8scd</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1ks8gvb</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Basic and short, but got my nails done at a salon for the first time, yayyy</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/som6mauu472f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1ks8ceb</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Gel manicure removed over a month ago and these are my natural nails…</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks8ceb</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1ks83x1</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>To be my third time making flowers, how do you think they were?🌺</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1i49tdu9272f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1ks8498</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>summer nails 🫶🏽</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks8498</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1ks8ad2</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Press on nails save my life</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/q2m26ezj372f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1ks8a88</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Pink on pink 💓</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks8a88</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1ks87kg</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ks87kg/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1ks7wl2</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Any Stays in the chat?</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks7wl2</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1ks7ncs</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Help, how can I stop my nails from curling?</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks7ncs</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1ks7eos</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>My new pink chrome nails 💕</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks7eos</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1ks6rod</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>obsessed w the light ombré that sheers give 🎀</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/niy0l8bns62f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1ks69s8</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Loving this nail and keyboard vibe</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks69s8</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1ks62kj</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Nail set I did for myself for my birthday 🎂 🥳</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks62kj</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1ks5uxv</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rxugfun4m62f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1ks51eh</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>What's your opinion on peeling-looking top coats?</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks51eh</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1ks4wcs</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>My new nails with chrome</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks4wcs</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1ks4xrt</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>✨🫧🦄🌸💖</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks4xrt</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1ks4wyf</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Recent Set!</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks4wyf</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1ks4gwz</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Sally Hansen Syrup - Pink Pour</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks4gwz</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1ks3xeu</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>love these nails but the opaque base coat is reeeally throwing me off and idk if i’m feeling it :(</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks3xeu</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1ks4r2o</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>want to get back into climbing and playing harp but also want nails.. any things to look for when getting press ons? recommendations? I've never used them before</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ks4r2o/want_to_get_back_into_climbing_and_playing_harp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1krom5n</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>What I asked for (bottom) and what I got (top) 🥰 structured gel mani by xoyanie</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zte4jb5y522f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1ks2068</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Any tips for 3D sculpting gel?</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bfbz7qbuu52f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1ks38t1</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>What shape suits my hands best?</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks38t1</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1ks2osr</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>My very first press on sets ❤️</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks2osr</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1ks2nou</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Spring nails 🥰🌷</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks2nou</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1ks2nl4</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Problemas con el top</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ks2nl4/problemas_con_el_top/</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1ks24n4</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>The coolest cat eye I’ve ever seen ✨</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks24n4</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1ks2247</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>New favorite pink</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks2247</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1ks1uda</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Peacock feather nails 🦚</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks1uda</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1ks1r95</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>I should’ve complained but I didn’t…</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks1r95</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1ks1q50</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>DND Periwinkle 😍</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4e2pnqvus52f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1ks1ori</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>New set for my Y2K themed bday party 🤩🤩🤩</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/39lh0emis52f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1ks1nna</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Summer lovin’</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks1nna</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1ks0qox</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>What nails would look good with my tattoos that’s not black?</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5s6p6j8ul52f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1ks0oo5</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Tried Doing cat eye nails , My brother said they look like witch nails are they bad ?</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks0oo5</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1ks0kp7</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Odd nails, press ons made by a coworker of mine</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/20lgtejnk52f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1krzq30</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>I wanted it to give ✨Barbie✨</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krzq30</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1krqa71</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Boards &amp; practicals</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1krqa71/boards_practicals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1krzu4f</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>new nails</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9pvped0gf52f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1krzi09</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>I hope Pedro Pascal likes this set</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krzi09</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1kryuo0</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Hannah Montana nails I did!!</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1gvg1w03852f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1kryo8o</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>I just did my nailssss</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ftr4zdnq652f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1krwztx</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>I need help!</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1krwztx/i_need_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1kryj9b</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>The vibes are immaculate</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kryj9b</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1kry5z5</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Love with this shiny purple</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7gtgodqs252f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1krxzrf</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Chrome wedding nails</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y8qbzk7e152f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1krxrri</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Summer fun!</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bz0tyi4mz42f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1krx4nn</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>I'm a guy and my female friends are jealous of my nails.</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zui1eb3bu42f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1krwubz</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>When Life Gives You Lemons...</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krwubz</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1krwqf3</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Is my biab/builder gel supposed to look like this?</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krwqf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1krvzqg</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Honeycomb summer set</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/08lihyd2k42f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1kruv4z</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Ombre and Aura</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kruv4z</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1krt94i</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Got my nails done and Mexico - so obsessed! 🤩</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ge94pcacp32f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1krt5d3</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Thoughts on my summer set?</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krt5d3</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1krszrp</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Apres Soft gel builder in a bottle</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z6ejovazl32f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1ksktwu</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Crème polish haul!!</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ikpc0vcda2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1ksjkg1</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>My comfort zone nail polish</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksjkg1</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1kshi8h</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>🌊Do y'all see my vision tho (crossposted! My first attempt at art)</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kshgyy</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1ksh70m</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Painted polish &lt;33</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/14wm2v0m792f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1ksg2r9</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Can i paint my nails as a guitarist ?</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ksg2r9/can_i_paint_my_nails_as_a_guitarist/</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1ksg0et</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>I suck at magnetizing</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksg0et</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1ksex9p</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Nail Polish ID?!</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksex9p</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1kseu9u</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>I can’t get enough of magnetic polish! 😻</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lwi37bmbl82f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1kseh9j</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Moon Spirit 🌙</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/aqvsrahzh82f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1ksearw</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Public Storage orange</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/heohs0bag82f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1ksdx01</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Nail down!</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hcj85i0sc82f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1ksdq9c</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Gimme all your tips for magnetic polishes!</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ksdq9c/gimme_all_your_tips_for_magnetic_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1kscfm3</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Mooncat dupes</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/87xri1dqz72f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1ksce3b</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>I Did Tell Myself I Wasn’t Going To Do Another Green…</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8myxwee9z72f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1ksbt2i</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Mooncat Donations Advertising is Sus</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ksbt2i/mooncat_donations_advertising_is_sus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1ksbs1q</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Layering polishes adds so much depth!</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksbs1q</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1ksbjxd</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Ethereal Beware faded already :/</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksbjxd</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1ksbjsl</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Ultrahot</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksbjsl</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1ksbiqz</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>OPI Ozitively Elphaba</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z4yy4vb3s72f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1ksb0uw</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Mooncat Castle of Cobwebs</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksb0uw</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1ksaemi</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Any nail polish in this shade?</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aftgwrd6j72f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1ksad1z</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Summer collections aren't giving</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksad1z</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1ks9lpt</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Ethereal / sheer budget polish comparison ✨</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks9lpt</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1ks9grc</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Nail polish noob, need shaping help!</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ztlzq55c72f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1ks8yzr</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Thistle and Thorn</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n94gtguk872f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1ks8vcu</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Sooo simple sooo in love</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks8vcu</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1ks8pl4</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Blinded by the sparkle ✨️</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks8pl4</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1ks8lxw</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Paint it pretty - Robin Egg</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gcm1ri4x572f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1ks8ghf</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Polish keeps peeling in full sheets regardless of what I use</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/77wdg22s472f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1ks8ef0</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>If you are a warm tone - Fool's Gold + Momento Mori is such a fun combo!</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9nil1snc472f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1ks8b4a</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Not My Best Application, But I Had To Show This Cute Color!</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks8b4a</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1ks7ij9</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>BKL Chaos - an unexpected new favourite!</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks7ij9</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1ks6xi6</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>What nail polish color goes with an alexandrite and rose gold ring?</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e9u0ww1st62f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1ks6wkn</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Ok, laqueristas … I may have actually found the closest shade match yet to Elysian Fields. Meet Candy Mayo’s 961</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks6wkn</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1ks6vy6</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Right hand today</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks6vy6</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1ks6msk</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>My left hand today😍</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks6msk</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1ks6jph</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Just wanted to show the difference..hope it helps!</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fyxj8902r62f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1ks6iy4</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>A super shiny orange!</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks6iy4</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1ks5s2b</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>💚💛 70s avocado green and gold kitchen vibes 🥑</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks5s2b</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1ks4oik</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>How do I fix my cuticles ? I already use an oil</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ahkc5o4rd62f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1ks45pv</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>My neon summer</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kteetyf3a62f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1ks3ctt</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Is There A Trick To Get The Extra Lacquer Off Before Next Slather?</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ks3ctt/is_there_a_trick_to_get_the_extra_lacquer_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1ks2yae</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>First time trying some actual art on my nails. Took like 4 hours 🫠</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks2yae</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1ks2sf6</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Ready for Summer 💙</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n83nmcaf062f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1ks2pu1</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Recently discovered Bee's Knees Lacquer</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks2pu1</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1ks2jej</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer swatch comparison</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/flcfay2ny52f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1ks2fwv</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Best black light polish/colors?</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ks2fwv/best_black_light_polishcolors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1ks28hh</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Notion Template Suggestions!</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks28hh</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1ks22a9</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Rainbow nails for my birthday 🌈</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nhdb9bp9v52f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1ks20q7</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>where can i find good magnets for nail polish?</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ks20q7/where_can_i_find_good_magnets_for_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1ks1s77</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Anyone have the capped edge of their nail just... Come off?</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s5q8dbc9t52f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1ks1he8</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Mooncat’s price jump</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ks1he8/mooncats_price_jump/</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1ks1by2</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>The Sweater Made Me Do It</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b3m6zy53q52f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1ks14jk</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Distance to the Sun - Emily de Molly</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yjkds0alo52f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1ks131h</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Stretching my mani a few extra days</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks131h</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1ks0mvp</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>My nails after being my friend’s caregiver for a week</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nxjuhra3l52f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1ks0g2f</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Beached Neons by Moonshine Mani</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/18j37c5rj52f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1ks0f4z</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Tell me your nail related stories please 🙂‍↔️</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ks0f4z/tell_me_your_nail_related_stories_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1krzw0k</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Sponge Jar refill?</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lj2gbvctf52f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1krzp2j</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Nail shape</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1zbk6q0ee52f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1kryrgv</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Wish me luck</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kryrgv</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1kryd68</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Tips for a bettet manicure?</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bi0v598f452f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1kry39r</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>My first ombré!</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kry39r</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1krwmox</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>anybody else's pinkie nails completely different sizes??</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hdofeb6xp42f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1krvv7t</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Cosmic Polish Wildflower Nights</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krvv7t</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1krvv1s</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>First try at ombré gel nails 🌸</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vkbaxoxsi42f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1krv2q3</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Unflattering nailpolish?</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gp7udussa42f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1krfd9c</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Dreamy lilac 💜</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4158vyhoyz1f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1krohiv</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>I can’t believe it’s not velvet</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3kw4vm3l422f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1krrkdu</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Cosmic Polish's Business End of a Broomstick from May 2025 Indies Down Under!</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1krrkdu</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1krts74</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Reflective Gel Polish Brands</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1krts74/reflective_gel_polish_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1ksk9qi</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Disney N ails!</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksk9qi</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1ksihpx</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Can anyone help me suggest a design/pattern for this?</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uj5yqzqcl92f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1ksgv2c</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Some nails I've done :)</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksgv2c</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1ksgc4l</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Nail embellishments??</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ksgc4l/nail_embellishments/</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1ksg81x</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>A little Barbie inspo</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksg81x</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1ksexms</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Had a fun idea for an aquarium nail inspired by Junji Ito and painted a lil set 🥰</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5wyu5go7m82f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1kseumd</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>just posting to help people that struggled with chrome</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kseumd/just_posting_to_help_people_that_struggled_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1ks996u</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Glitter ombré nails with fun fruity designs!</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks996u</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1ks8jig</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Abstract 3D</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ag1szve572f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1ks7w9y</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Still getting the hang of diy</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9mjgcjfr072f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1ks77bf</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Flowers</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hymocojsv62f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1ks69hl</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>what nail polish gives this effect?</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks69hl</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1ks44fc</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Spring Nails done by me on a friend 🥰🌷 - unsure of original artist, inspo at the end</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks44fc</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1kryx39</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>first timer nt</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kryx39/first_timer_nt/</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1kry3r5</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>First try at aquarium nails</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kry3r5</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1krxa6s</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Gel nails in India</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1krxa6s/gel_nails_in_india/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri May 23 08:12:31 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_05_25.xlsx
+++ b/data/collected_data/2025_05_25.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C843"/>
+  <dimension ref="A1:C1033"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14764,6 +14764,3236 @@
         </is>
       </c>
     </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1kte514</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>questions about gel nails</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kte514/questions_about_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1kte4t1</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>summer nails 🐆</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kte4t1</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1ktd8qw</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>What is the use of “Solid Nail Tip Gel”?</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ktd8qw/what_is_the_use_of_solid_nail_tip_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1ktcyou</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>My new nail tech is the besssst</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t3xnbb0x9h2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1ktcsw7</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Cute Press Ons 🖤</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ecgvok108h2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1ktc82n</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>My Micro watercolor painting set</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ojpyryl31h2f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1ktbtjp</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Pink Halo Donut glaze 1st attempt</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lw1lvuubwg2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1ktbpe8</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>I got them done a week ago but I’m still obsessed</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8sb0qdvyug2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1ktbne9</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Just a straight man that took his mom to get her nails done and got his first manicure. Charcoal matte. 💅</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kqld23dcug2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1ktbkly</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>forever obsessed with my natural nails even tho they’re never the same length</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktbkly</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1kt8vbd</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Couple questions</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kt8vbd/couple_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1kt9bxg</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Independent Artist</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kt9bxg/independent_artist/</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1ktav7n</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Fun sets from this week hehe</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktav7n</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1ktad7j</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>geek out with me for these kirby nails</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktad7j</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1ktaav2</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>geek out with me kirby nails for my daughter's birthday</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktaav2</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1kt9mbo</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>First try. Monet nails.</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o2n2xds99g2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1kt9if9</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Sooo cute</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/c1ekkpa78g2f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1kt9ea8</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>I really miss my nail master</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt9ea8</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1kt878d</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>porcelain nails</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fhumxxyovf2f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1kt8hxv</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Tried press on nails for the first time</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt8hxv</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1kt8gbn</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Dip powder nails, third attempt with better quality supplies</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt8gbn</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1kt8csy</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>I don't think I will get sick of doing cat's eye + isolated chrome combos</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9p8aiv34xf2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1kt87dr</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Decided to try something new💕</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0shf5xlpvf2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1kt7zw1</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>First Gel X set on myself!</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt7zw1</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1kt7xex</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>I was supposed to wait until june for summer nails but....</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt7xex</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1kt7vav</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>broke a nail and now i have to file them all down :(</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6e8xog0nsf2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1kt7tfb</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>summer/bday set!! (srry the pic sucks😭)</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nocejxd5sf2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1kt7nou</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>I call this ✨flower power✨</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ev3hgfyoqf2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1kt7kwu</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Should I ask for a refund tomorrow 😭</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt7kwu</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1kt7fei</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>First time trying paintlab</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt7fei</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1kt78dh</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>My girl killed it!!!</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mffknmkqmf2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1kt7206</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>whats the trick to making cuticles look good</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ql18yuqxkf2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1kt6po8</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Brittle Nail Recovery</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kt6po8/brittle_nail_recovery/</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1kt5xwo</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>KISS sticky tabs stick to fake nail??</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/temv11zraf2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1kt5wh9</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>What are your tips to make press on nails look more natural ?</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kt5wh9/what_are_your_tips_to_make_press_on_nails_look/</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1kt5piw</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>i didn’t love what i walked out with. inspo from @basecoatstories</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt5piw</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1kt5lck</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>OPI - Blew Them Away</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt5lck</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1kt5hxj</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Diy polygels</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3lsg0d4x6f2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1kt5er4</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Planting Inspo</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t5x1tzs56f2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1kt572c</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Deer spot nail art</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wxb9w4ab4f2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1kt4rn3</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>@ Pressed.pretty.by.hails on IG</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt4rn3</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1kt4xng</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Oval nails… wtf is this.</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/imctnus12f2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1kt4ajh</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>I need help to remove press on nails!</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt4ajh</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1kt4ch3</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Just got my nails done less than a week ago and they already look weeks old?</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t3gksxw4xe2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1kt42l3</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Nail injury, can I get gels?</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kt42l3/nail_injury_can_i_get_gels/</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1kt454r</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Low to no damage nail options</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kt454r/low_to_no_damage_nail_options/</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1kt43x4</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Something Blue for my Bridal Shower</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt43x4</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1kt2lhc</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Should I be upset about the shaping of these nails?</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt2lhc</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1kt3l7e</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>want to get into nails please help me :(</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kt3l7e/want_to_get_into_nails_please_help_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1kt3ib4</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>ALMOND SHAPED RUSSIAN MANI IN AN OMBRÉ FRENCH 🤍</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p9ufxns9qe2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1kt3fzh</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>🖤</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt3fzh</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1kt34jl</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Feeling fresh and a little grungy with these nails 😤</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt34jl</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1kt31jd</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Moonlight chrome I did for my dissertation defense! 😍 Now a nail girlie, PhD. 💅</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt31jd</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1kt2twe</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Is my nail lifting?</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/prbra8i2le2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1kt2kpo</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>How to identify flooded cuticles in pictures/videos when looking for a nail tech?</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kt2kpo/how_to_identify_flooded_cuticles_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1kt1pw5</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>This is my last time visiting a nail salon - always disappointed</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt1pw5</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1kt242v</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>My long stiletto client is back!</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt242v</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1kt1pok</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Newest DIY Set</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt1pok</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1kt1483</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>something different 🌸🖤</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dt22tjfg8e2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1kt1111</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>SpongeBob nails for my birthday!!</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b6ojvv2t7e2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1kt0ws9</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Removed my builder gel manicure at home. Only took 1.5 hours because my soak off remover was nottttt strong enough. I need a serious buffing now. Only one nail is thin and flexible at the tip so I am trying to protect it 🥲</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt0ws9</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1kt0vg8</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Not so Mellow Yellow</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ec6z71yp6e2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1kt0i68</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>How to do a glitter fade tip without the tips being way thicker than the rest of the nail?</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt0i68</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1kt0fmu</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>My first set!</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jiibx6sk3e2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1kt0ck9</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>advice needed</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt0ck9</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1kt0caj</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Love days</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt0caj</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1kt02hi</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Amalfi-inspired BIAB 🍋</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lo20hedx0e2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1kt064o</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>In awe of what my friend can do with my nails</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt064o</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1kszs1m</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>How are these looking?</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/esej757ryd2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1ksz4vb</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>I wanna get back into doing my nails</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ksz4vb/i_wanna_get_back_into_doing_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1kszdco</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>I AM  IN  L❤️VE!!</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jvilx4zsvd2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1ksyx0r</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>french tips! did them myself 💗</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gmlv0o4ksd2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1ksype2</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Love this set</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksype2</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1ksypd9</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>My right middle finger is so rough :(</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksypd9</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1ksygdy</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>brat summer forever (by Jocelyn @ Get Nailed)</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksygdy</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1ksy9k0</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Where can I find charms like these</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1pyeiazsnd2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1ksy371</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>I dare to let them grow a little 😁</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rcbhdwdjmd2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1ksxzn1</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Fresh Set 🩵</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oofrap7tld2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1ksxszv</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Summer nails 💅🏼</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksxszv</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1ksxdnh</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Hello Kitty Nails</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1z3seosghd2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1kswupy</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>“I really should try out those stickers I bought 3 years ago”</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kswupy</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1kswrrf</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Is the natural length/durability good enough to take off acrylics?</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kswrrf</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1kswnsr</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Today's nails</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qt19dkjbcd2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1kswjxg</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Y’all the perfect neutral</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kswjxg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1kswb57</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>My new nails!</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kswb57</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1kswfgj</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Kiki delivery service nails</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kswfgj</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1ksvyg4</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Spring set.</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/691w0wtd7d2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1ksvx7b</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>help with blooming gel!!!!</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksvx7b</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1ksvp1t</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Nail Hardeners &amp; Nail Care</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ksvp1t/nail_hardeners_nail_care/</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1ksqf8q</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>I broke a nail! Help!</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6aj65yis2c2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1ksosqe</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>nails flaking/splitting under biab</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksosqe</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1ksu8zx</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Memorializing this set before I have to take them off. Found out I’m allergic to acrylates 😔👎🏻</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksu8zx</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1ksvile</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Polygel Starfire pink nails</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksvile</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1ksvbmi</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Press on nails</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksvbmi</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1ksv4c1</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>In love 💖💖</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0lzoiste1d2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1ksuo9j</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>It is the first time i used cuticule softener for my manicure, I'm quite happy with the result!</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bezburj8yc2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1ksu40v</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>At home gel only lasting 1-2 weeks</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ksu40v/at_home_gel_only_lasting_12_weeks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1ksu3i4</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Classy French tips</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cshljh36uc2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1ksteci</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>What u think?</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qvgiz4c2pc2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1ksg2l6</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Help! How to fix this cracked nail?!</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dkojgzvtw82f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1kte0b3</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Grey/red multichrome?</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kte0b3/greyred_multichrome/</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1ktcbns</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Fair Isle over purple!?!?! 😍</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktcbns</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1ktc10x</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Bee’s Knees Lacquer Lion Sibling Appreciation Skittle.🌈</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i7lwuvyqyg2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1ktbpyi</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Fancy vs Get Lobstered vs Fairycore</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/155akz15vg2f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1ktbit7</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>I changed the shape of my nails and cannot stop staring at them now!</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktbit7</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1ktaqxy</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>A-Z challenge</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktaqxy</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1ktanxm</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>J&amp;B - Lilac Arches 🫶</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktanxm</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1ktancl</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>No one in my life appreciates how much of a personal flex this is.</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktancl</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1kta91z</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Gracie Jay &amp; Co. not shipping orders and ghosting customers.</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kta91z</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1kta43t</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Need advice! Overfiled nails?</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d4ym49j2eg2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1kt9vo9</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Nail polish over other alternatives</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kt9vo9/nail_polish_over_other_alternatives/</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1kt9nw9</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Buckle Up! This shifty purple is almost here!</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt9nw9</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1kt8xbz</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Purple skittle</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt8xbz</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1kt8qwp</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Dupe for Revlon Provocative?</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nxzi4kdo0g2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1kt7pm8</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Recs for male-friendly salons in Northern Virginia?</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kt7pm8/recs_for_malefriendly_salons_in_northern_virginia/</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1kt7468</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Anyone got any dupes for this shade from Olive and June?</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n1jcw5imlf2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1kt6r09</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Dazzle Dry Cupid's Arrow</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r7ysdaurhf2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1kt6f81</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>My 75-year-old dad over here showing off his mani on facebook for the first time!</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1vxsttc5ff2f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1kt6e78</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Happy Accident skittles</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt6e78</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1kt5ws6</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>First multichrome</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt5ws6</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1kt5vxq</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Dupe for this Dark Indigo gel?</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zt7vj3raaf2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1kt5fu6</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Just can’t get enough! ✨✨✨</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8e2xkrye6f2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1kt53f9</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Shimmer Topper Recommendations</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kt53f9/shimmer_topper_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1kt4s63</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Sparkliest ever</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt4s63</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1kt3tb2</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Thank you for the advice !</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt3tb2</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1kt3n82</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Fairy Ring 🍀🪲🪻🧚‍♂️</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a9cf26gcre2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1kt3lkw</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Photos never do my colors any justice.</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gjsbw72zqe2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1kt3ju7</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>ILNP - Deep Space 🌌</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n056vlslqe2f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1kt31o2</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Darth Vader On Edibles</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt31o2</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1kt2qy9</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer- Barbed Beauty</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt2qy9</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1kt2hsa</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>why didn’t anyone tell me that layering polishes would be this fun?!</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt2hsa</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1kt255q</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Granite Daisies (Tenacious Weeds)</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt255q</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1kt1zqm</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>my favourite pink 💕</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt1zqm</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1kt1o60</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>How long will my chrome powder/UNT ready for takeoff nail lasagne take to dry...?</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kt1o60/how_long_will_my_chrome_powderunt_ready_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1kt1abw</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Nail polishes with similar formula to No7 Gel Finish?</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt1abw</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1kt0k1f</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>WE ARE LIVE!! 🎉🎉🎉</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kt0k1f/we_are_live/</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1kt0iw4</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Baeocystin Troubleshooting</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9oerq4o04e2f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1kt0gnb</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Thoughts on toluene?</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9n1j2dur3e2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1kt00ur</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Fav Zoya cremes?</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kt00ur/fav_zoya_cremes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1kszfnd</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Atomic!</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kqr1p2q9wd2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1ksz6hd</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>KART Pedicure Reviews?</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ksz6hd/kart_pedicure_reviews/</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1ksz2jy</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>🌸 spring vibes 🌸</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksz2jy</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1ksyxp1</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Which brand is great for one coat cremes?</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ksyxp1/which_brand_is_great_for_one_coat_cremes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1ksyp8r</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer - Blood Bag 🩸🎒</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jmgg6i91rd2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1ksyd9w</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Moonlit Rodeo vs Wallflower</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ksyd9w/moonlit_rodeo_vs_wallflower/</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1ksy9ro</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Love this combo</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksy9ro</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1ksxp3r</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Cracked Polish subreddit?</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ksxp3r/cracked_polish_subreddit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1ksxhel</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Painting my nails to cope with current events…anyone else?</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksxhel</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1ksxdrk</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Looking for new indie brands to try! What are your favorites.</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ksxdrk/looking_for_new_indie_brands_to_try_what_are_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1kswqb4</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Playing with layering polishes</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kswqb4</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1kswgb5</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>I chipped yesterday,s mani so did another one today and look so pretty</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0cirxy9sad2f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1kswa9b</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>What causes these bumps I sometimes get in my nail polish?</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wktk322o9d2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1ksw9w8</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Rose Cappuccino 🌹</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksw9w8</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1ksw4yr</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Moonbeams &amp; Magic!</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksw4yr</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1ksvzd3</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Toppers over naked nails 💅</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a6vlwj9k7d2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1ksvrve</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>🌿mint mojito🌿</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksvrve</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1ksvrs6</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Essie - Birthday Girl</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksvrs6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1ksuzzt</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Cracked Polish</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ksuzzt/cracked_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1ksuryc</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Crone claws</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k19cgrmyyc2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1ksuibk</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Recommend a polish?</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zb762r0twc2f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1ksudqh</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Tri-Thermal Flakie Magic</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksudqh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1ksu3x6</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Bee's knees Baldur's Gate 3 -Astarion Edition</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksu3x6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1kstylg</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Nail Bed Shape?</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kstylg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1kstpid</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Jade Jelly</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kstpid</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1kstixt</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Is "Frolicking in the Fields" from Cracked a good dupe for Mooncat's "After the Rain"?</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kstixt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1kstga3</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Advice for shattering, flakey nails?</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kstga3/advice_for_shattering_flakey_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1kstf2p</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Magical Flowers 🌸</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kstf2p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1kssjp7</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Some favorites from Cracked 💚🩵🤍</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2bw862owic2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1kss6kw</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Base/nude recco for French tips</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kss6kw/basenude_recco_for_french_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1ksqo6k</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Slept on this Lion Cousin a little too long</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksqo6k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1ksptzi</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>After 4 months of fighting peeling, breaking nails, I finally feel confident to show off my natural nails 🥳</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o0b33ahuxb2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1kspqre</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Life After Beetles?</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kspqre/life_after_beetles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1kspbwr</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>what’s wrong with my nails??</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kspbwr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1ksp4mj</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Searching for 'soft' holos</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksp4mj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1ksowim</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>I went to a sweets-themed costume event this week and I'm so happy with how my nails turned out! Can you guess what my inspiration was?</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/86wy8ttipb2f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1kskecz</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Hey friends! Looking for topcoat advice.</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kskecz/hey_friends_looking_for_topcoat_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1ksogdh</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Making my own stamping plate</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ksogdh/making_my_own_stamping_plate/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1ks6tu3</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Question re: Chamaeleon Nails</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ks6tu3/question_re_chamaeleon_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1ks74s2</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Worth it!</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ks74s2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1ksocs9</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Sally Hansen Vit E Nail Oil Still Okay After Years of Not Being Used</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>/r/Nails/comments/1kqvj07/sally_hansen_vit_e_nail_oil_still_okay_after/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1ksn8ue</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Was in dire need of a palate cleanser - here we go with sand boomer</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ksn8ue</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1kt9syf</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Blueberry set for May</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt9syf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1kt9eba</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>I’ve been practicing nail art for a year now and did this set tonight</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt9eba</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1kt9cah</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Coca Cola labubu nails 💅🏼</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt9cah</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1kt9aoz</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>That reminds me of driving lessons.</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h0tytip26g2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1kt6rhm</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Crosses</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt6rhm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1kt2edd</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>How to create 3d flowers without a silicone brush</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9am3090rhe2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1kt1gtj</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>shorties</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt1gtj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1kt07og</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Love days</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kt07og</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1ksnegx</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Black and champagne nails</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/id5djc0v9b2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat May 24 08:10:16 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_05_25.xlsx
+++ b/data/collected_data/2025_05_25.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1033"/>
+  <dimension ref="A1:C1224"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17994,6 +17994,3253 @@
         </is>
       </c>
     </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1ku5ikr</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>My first go at Gel-X 🍒</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tfu2k0fmho2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1ku4u6p</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>What do you’ll think? 💅</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ku4u6p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1ku3tcg</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Best shape for me?</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ku3tcg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1ku3szc</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Transfer foil beginner here.😅</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7b9wcu2dxn2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1ku3o3d</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Tangled Nails 😍</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ku3o3d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1ku1tsc</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>10/10 design but she ruined the shape</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n0e7jcbccn2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1ku1y7a</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>i did my own nails for the first time :)</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/56mdyszjdn2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1ku1sk1</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>almond or round?</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ku1sk1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1ku1ah6</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Product advice needed</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/az3kn1jy6n2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1ku0f9r</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Assistance please</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ku0f9r/assistance_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1ku0nmv</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Shaken, not stirred 🍸💅</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h2tatt1n0n2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1ku0mom</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Lucky Red, my fav color</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wiq7jt4e0n2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1ku0e1c</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>🤍🩷</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ku0e1c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1ku0b5l</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Girls, How is better? Almond or Square</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ku0b5l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1ku002u</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>So excited for my goth nails!</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ku002u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1ktvvnl</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>First time doing my own press ons. Questions about fit.</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktvvnl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1ktzlap</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Engagement Nails</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ou9pmv4gqm2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1kty4g8</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Press on nails</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kty4g8/press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1ktzl1h</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Got nervous and changed my mind half way through lol</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktzl1h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1ktxun2</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>How can I make these more cohesive?</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktxun2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1ktzffc</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>😍😍</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7duosq4xom2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1ktyp2u</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>How to take false nails off?</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ktyp2u/how_to_take_false_nails_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1ktynxb</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>What are some good cat eye nail polishes?</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ktynxb/what_are_some_good_cat_eye_nail_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1ktyf16</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>How often do you actually get a whole new set for acrylics?</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ktyf16/how_often_do_you_actually_get_a_whole_new_set_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1ktye53</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Need advice with glue on extensions</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ktye53/need_advice_with_glue_on_extensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1ktyd6u</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>New nails must mean it’s holiday time 🍊🍋</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktyd6u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1kty1mk</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Does anyone own one of these and would you recommend?</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ys3r8hv6cm2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1kty1jz</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>So cute</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f435wtc6cm2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1ktxxka</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>New tech delivers</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktxxka</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1ktxt1p</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>First time gel nails and cat eye!</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8tghptp1am2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1ktxm84</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Square or almond</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iup6nt8e8m2f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1ktxbjw</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Because it is summer time!!</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktxbjw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1ktwxvb</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Press On Tips</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktwxvb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1ktwsgw</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Do u love it?</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ifqxjlpb1m2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1ktwlvt</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>melody susie not curing</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ktwlvt/melody_susie_not_curing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1ktvxkw</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Polygel nail attempt</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/davm6ea5ul2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1ktvu3v</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Just finished my first week of nail school!! I’m so excited to be getting certified!</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktvu3v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1ktt19y</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>New to gel- what do I ask for?</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/thcdsh8u7l2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1ktu443</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Can I put paint my nails?</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktu443</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1ktv1rv</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>How do you guys remove glue on/press on nails?</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7979qva7nl2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1ktvpjm</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>simple butter yellow</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wmeaw51esl2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1ktt0vc</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>so sad</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/74hbxw3r7l2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1ktvpbd</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Being basic 💅</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o3aiyamcsl2f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1ktpn09</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Silly art</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktpn09</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1ktvc6x</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Parttime job</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ktvc6x/parttime_job/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1ktv2g4</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Ideas to improve</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktv2g4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1ktv10m</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Can i switch directly from acrylics to gel?</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ktv10m/can_i_switch_directly_from_acrylics_to_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1ktuzo2</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>I just finished getting my new nails done 💖 do you like them?</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dn25jypqml2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1ktux8f</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>nails done by me 🤎</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktux8f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1kturk9</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>I want to change my nail color, what do you recommend? 👀💙</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ggcwjttzkl2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1ktufxw</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Electric Forest festival nails</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktufxw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1ktudvk</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Finally got my nails thick and long after years of biting</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v0xgfjb4il2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1ktucu3</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>My natural nails have grown since using GEL X</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktucu3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1ktu4dk</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Did these kawaii nails at home w diy gems 💖</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ngumuh3sfl2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1kttvb2</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Perfect Match #243 Tell Me Lies polish match??</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kttvb2/perfect_match_243_tell_me_lies_polish_match/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1ktttyw</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Hi girl 1 or 2?</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktttyw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1kttnum</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>did my first polygel set by myself!</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ffu10nqjcl2f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1kttipy</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Mediterranean vibes</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vtsrtkogbl2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1ktthid</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Shellac natural nails roundshape</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ew0nbuh7bl2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1kttfak</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Hands ready to subdue you</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/addn9j0qal2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1kttevq</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Getting ready for pride next month!!</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kttevq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1ktt8ly</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>all my students said blue!</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktt8ly</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1ktt7p5</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>PROM NAILS!!! 💕</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nd941c659l2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1ktt4wi</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Citrus 🍊 🍋</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jq64ylak8l2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1ktsyle</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>No idea where to start!!</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktsyle</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1ktsxv1</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Are they too christmas-y?</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ufyod0737l2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1ktssam</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>decal set i did today</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktssam</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1ktsjad</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>🐸🐸</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktsjad</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1ktshuh</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Snorkeling vibes</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cfzpi62o3l2f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1ktp0w5</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>birthday set!</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pxlirts9ek2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1ktr0wt</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Should gel be falling apart this fast?</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktr0wt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1ktrc1c</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>🌸 Summer Nails 🧡</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktrc1c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1ktr2ec</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>anyone know how to strengthen my nails?</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ktr2ec/anyone_know_how_to_strengthen_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1ktqtp6</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Some of my recent nails by my amazing nail tech</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktqtp6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1ktqpvf</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Question on coverage</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8sfh0ydgqk2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1ktqige</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Do I have Ski Slope Nails?</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktqige</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1ktpxvl</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>let’s play a game &lt;3 guess the price for my birthday nails!</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktpxvl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1ktps2c</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>I think this was definitely worth 60$</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wz11jkdmjk2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1ktpope</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Love my new ones 💕</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktpope</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1ktpmm8</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>nail update</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hq7ammriik2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1ktp8no</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Totally forgot to post these when they were new</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktp8no</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1ktp62g</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Totally forgot to post these when they were new</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktp62g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1ktoxu5</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Need a New Salon</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ktoxu5/need_a_new_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1ktopz0</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>One of my nails came off and…</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f665s074ck2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1ktorpb</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>what do we think</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zlicj0egck2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1ktnpmq</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Question: How to get nail techs to stop making me bleed?</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ktnpmq/question_how_to_get_nail_techs_to_stop_making_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1ktoodr</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Pink chrome💗💕</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jb7u9pdubk2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1ktoo7i</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Pink chrome💗💕</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/809x12vsbk2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1ktog85</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Tried chrome for the first time!</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktog85</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1ktofbo</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>new nails!!</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sy5xa9xz9k2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1kto7rx</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Got these done yesterday!</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kto7rx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1kto5q9</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>This might be a dumb question but…gel tips?</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kto5q9/this_might_be_a_dumb_question_butgel_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1kto1uy</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Got my nails done 🙌</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3lexgw8a7k2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1ktmjr7</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Too thick with too much space at the cuticles?</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktmjr7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1ktn98x</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Looking for nail techs/salons recs in NYC area</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ktn98x/looking_for_nail_techssalons_recs_in_nyc_area/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1ktn2f2</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>My most favorite red. ILNP-Sabrina</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktn2f2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1ktmrh4</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Made my first press on nails!</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/74a79hduxj2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1ktmj74</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Help with sizing</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n1kd7tv7wj2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1ktmccb</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>My pastel, unicorn nails! I think I’m in love with these! 🤍🦄</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktmccb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1ktlvy5</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Heading to the Cowboy Carter tour this weekend 🤠</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fj3l4pvhrj2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1ku69j8</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Any dupes for these two polishes?</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ku69j8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1ku51be</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Green/Gold Metallic?</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ku51be</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1ku4b1z</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>(tmi/tmo) would it be crazy to buy 11 polishes from a brand i've never tried before? (Cracked)</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jwnsi9123o2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1ku3mq5</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Been a long time since I did my nails, so happy with them</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f6345jhevn2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1ku32s8</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Neon Shimmers</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ku32s8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1ku23tl</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Cutesy manicure 🍓</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ku23tl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1ku1z40</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Hanami "Magic" Set</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ku1z40</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1ku1cg6</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>i did it! i found my saturated blue!</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ku1cg6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1ku0zcc</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Cherub in her natural habitat🩵 (swipe to see a messy nursery)</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ku0zcc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1ku0p9b</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Even the Penguins Are Pissed</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ku0p9b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1ktzws5</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>How do I prevent this with magnetics?</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktzws5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1ktzh5c</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>HELP—I need detailed, step-by-step instructions for cuticle care. I’ve been ruining my nails without realizing I think.</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/efrsnfhdpm2f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1ktzewc</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>ORLY has an arcade now??</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktzewc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1ktzeiz</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Uno Mas Colors restock - May 24th at 1pm PT!</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktzeiz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1ktywe6</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>💅 Buckle up, Bitchlings by Sassy Sauce</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktywe6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1ktypx3</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Metallic lilac/lavender</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktypx3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1ktykin</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Spring gargoyle nails💚</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktykin</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1ktycry</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>OMG I LOVE ARIEL!!!!!!</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktycry</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1kty912</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>What are some polish yall recommend ?</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z6avjhq2em2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1ktxpmn</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>well, I guess I’m a flower child now 🌺</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktxpmn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1ktxnu9</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Quick before it spreads!</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xy77dwds8m2f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1ktxd0v</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>From my first PPU order! March 2025!</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktxd0v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1ktx9ea</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>BKL Patroness of 🐱 ✨</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktx9ea</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1ktwt15</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Novice Needing Help</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ktwt15/novice_needing_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1ktwsz9</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>ideas for nail-themed gift basket?</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i0r4996axl2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1ktwlbr</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Mod Applications! Looking for people in the Western hemisphere</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ktwlbr/mod_applications_looking_for_people_in_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1ktwkhg</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>ILNP Glass Candy causing bubbles</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktwkhg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1ktvbhk</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Marketplace temptation</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rogdg8lapl2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1ktujdp</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>I love this polish so much! 😍</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktujdp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1ktui5x</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>*screams from the top of a rooftop* I LOVE THIS COLOR!!!!!!</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yepn8k9zil2f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1ktu74g</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Out of my comfort zone but we’re here 🦋</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cg3tyc7ogl2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1ktu3ol</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Crochet Insperation</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktu3ol</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1ktu12h</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>File or clip toenails?</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ktu12h/file_or_clip_toenails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1kttxbi</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Found this at Marshalls for $4.99...</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kttxbi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1ktt8lw</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>non-thermal/magnetic polishes with this vibe? i’m in love with the color combo 💔</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zjvuhxqb9l2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1ktt8kr</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Death Valley Nails — Viva la Frida</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktt8kr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1ktsv4n</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Jelly sandwich: Spring Pastel Alien Egg edition</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t0b1o8kw5l2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1ktsuqv</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>My first Cirque Colors order!</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nvlbf3be6l2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1ktsiqg</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>I found my perfect match!</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c0btarhu3l2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1ktsiod</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Don’t you know you’re toxic?</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktsiod</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1kts7ec</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Memorial Day Mani</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l3r9kkge1l2f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1ktru99</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>so shimmery ✨</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktru99</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1ktrgk4</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>ILNP Butterflies and Cracked’s Rocky Mountain Iris?</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ktrgk4/ilnp_butterflies_and_crackeds_rocky_mountain_iris/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1ktrfyt</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Probably my favourite polish ever</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktrfyt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1ktrar7</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>In the wake of price increases, just wanted to share that Cirque is having a sale today!</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/62gkppdquk2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1ktr2ud</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Obsessed with Silent Library</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ggly7944tk2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1ktqf9y</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Non QDTC still ruined after 3 hours of waiting</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pq8qai6bok2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1ktqbqs</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Can we achieve this with regular magnetic nail polish?</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktqbqs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1ktpb9j</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>ALIEN INFATUATION 👽 🧟‍♀️</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktpb9j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1ktp1nv</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Gel allergy recovery</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktp1nv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1ktotk2</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Rue Morgue</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktotk2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1ktod20</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>First gel manicure for bridal nails - eye reaction.</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jfv2nujj9k2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1ktnvhd</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Lurid - Purple Eyed Shadow Daddy (velvet) &amp; Stargazing on Solstice</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tkhjl3wy5k2f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1ktn2wa</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Purple shimmer and reflective glitter? YES PLEASE!!</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m2lysxn50k2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1ktmyoe</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Glow Succ-ah by Sassy Sauce Polish goes live today!</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jb9f9wjazj2f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1ktmlsv</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Lurid’s Pissed Off Polishes of the Month: Fired Up!</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktmlsv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1ktmkbj</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>This changed by brain chemistry 😯😵‍💫</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7g3vufrfwj2f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1ktmede</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Right when I finally got my shape perfected</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tk63g0o8vj2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1ktloib</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Sparkling sand💖</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fhklmue1qj2f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1ktle1s</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>We need to talk about Danglefoot</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktle1s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1ktl1un</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Kidnap A Mafia Boss</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktl1un</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1ktkyf8</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Dupe request / Do PPU shades ever restock?</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktkyf8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1ktjfzj</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Lurid is absolutely the master of greens 💚💜💚</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ce1dhs6s8j2f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1ktip9u</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Here Comes the Smolder</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktip9u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1ktilxh</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Turquoise and Silver Shine</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktilxh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1ktihzy</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Home Gel UV kit for beginners? Which brand?</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ktihzy/home_gel_uv_kit_for_beginners_which_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1ktib8a</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Soooo many rainy days, so I did flowery nails 💐</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uaz9zda8zi2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1kthx2w</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>What is your Nail Nemesis?</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/umgme72rvi2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1ktgsng</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Thought I'm gonna hate this but this is actually really pretty 😍</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktgsng</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1ktg2qe</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Why is my gel polish uneven?</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/47wxii3zci2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1ktecwt</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Are salons supposed to remove gel like this?</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gpf88djhrh2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1ku52hl</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>One of my Favourite Sets I've done</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nhdt9ou4co2f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1ku1xfu</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>recent nails🖤</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ku1xfu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1ku04kh</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Beginners Need Appreciation</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xsld4m2lvm2f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1ktzwpb</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Just finished my Beyoncé cowboy Carter nails!!!</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktzwpb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1ktyy73</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>what did i do wrong</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktyy73</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1ktuwso</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>🍰(sanrio-ish) sweets-themed press-on set🍮</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktuwso</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1ktupqo</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Medieval Desert Spice inspired set</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktupqo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1kttur0</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Birthday Nails!</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kttur0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1ktts50</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>These are from today, what nail glue is best for press ons? I’m currently using glamnetic and I hate it 🥲</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lhj19ougdl2f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1kttqgw</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Trying to get better</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vikqhea4dl2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1ktt9sf</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Tips on how to achieve an ombré?</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j9jbhpyj9l2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1kts5uy</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Black &amp; White ➡️ Rainbow</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y2cvy5b21l2f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1ktpcea</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Line art colors bleed into each other</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/et8kboohgk2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1ktp99d</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>My nail tech did her thing again!</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktp99d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1ktnq9d</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>capybara nails</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6vj4yamw4k2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1ktnd3o</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Beautiful mom's design</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ey7yygl72k2f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1ktmgem</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Mean Girls press ons for my classmate!</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ktmgem</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1ktlhmh</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Graduated yesterday, these were my grad nails!</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vcvfpqfnoj2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1kth9rb</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Got my nails done for the first time ever... I'm obsessed 🖤 (@luxtrendnails)</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kth9rb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1ktfzsi</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Beautiful ombré and pearls @sueznails</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s3t4dmv0ci2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun May 25 08:10:49 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_05_25.xlsx
+++ b/data/collected_data/2025_05_25.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1224"/>
+  <dimension ref="A1:C1414"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21241,6 +21241,3236 @@
         </is>
       </c>
     </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1kuwmew</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>doodled on my press on nails</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuwmew</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1kuwkki</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>This is my favourite picture of a set I’ve done, this set was on myself</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x9tfkiugov2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1kuv3tb</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>rip the natural set</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuv3tb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1kuw8jj</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Summery nails. 🪻</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuw8jj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1kuvx7y</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>These give me summer vibes 💅</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gmkejq4mgv2f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1kuvusf</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Neutral makes me happy!! 🥰</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/33yb6oyqfv2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1kuvi4n</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>I’m halfway through nail school. I just did this fun set on myself &amp; wanted to share :)</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuvi4n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1kuv709</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>How much u would you pay for these?</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuv709</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1kusskf</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Nail tech conversation</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1dojd32ohu2f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1kutsr4</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Ersa nails vs Nail Witches?</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kutsr4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1kuub0t</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Made my nails today</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuub0t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1kuu00h</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>This is another one that I once had, I like to make different designs.♥️</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0sqk8bgguu2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1kutzeo</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>This design drove me crazy, since I saw it 😍😍</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fk6om4v9uu2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1kutxkr</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>New design, what do you think?</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y414w07qtu2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1kutu8v</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Need help identifying the middle nail polish</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lcwgowdrsu2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1kutsu3</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Neon strawberries 🍓</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wcn9i2ubsu2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1kutmaj</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>New Set - Different for Me</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ba3n4dfqu2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1kutgzj</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Airbrush alcohol inks not working?</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kutgzj/airbrush_alcohol_inks_not_working/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1kutgiv</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>First time with chrome nails and I'm loving em!</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mrzstw7nou2f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1kute3h</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Ready for my new set of nails. Should I stay with almond or go for something else?</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ry9ycywnu2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1kut07i</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Fairy core 🧚🏾‍♀️</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kut07i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1kuspb0</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Almond vs Stiletto?</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuspb0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1kusmba</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Nail etiquette question for pros</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kusmba/nail_etiquette_question_for_pros/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1kusc1e</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>first time trying almond</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kusc1e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1kus3yh</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Are these gel or acrylic</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oi8361hlau2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1kus34w</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>How much would pay for these two sets?</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kus34w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1kurz4c</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>I usually do my own nails but went to get them done before a trip 😊</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lq7e2rv89u2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1kury0j</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>First time getting my nails done &amp; I'm in love!</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kury0j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1kurvks</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Do nail salons cut your cuticles or push them back?</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kurvks/do_nail_salons_cut_your_cuticles_or_push_them_back/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1kurpob</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Which set should I choose? Nails credit in description!</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kurpob</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1kur6k1</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Alternative for Acrylic Nails</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kur6k1/alternative_for_acrylic_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1kurdza</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>French</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h0lkh03a3u2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1kuqvgx</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>what do you think?</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuqvgx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1kuqsi6</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Annoyed that they don’t go all the way to the cuticle.</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1n8nulicxt2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1kuqou6</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Possible proposal nails</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1n2pvy4bwt2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1kuqg4v</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>I bite my nails. What to ask for?</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuqg4v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1kuqk75</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Love fresh nails! 💕</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pj1v2urzut2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1kuqgu2</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Thoughts on my nails? I did them myself</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1421ua22ut2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1kuqcpd</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Gel polish possible allergy advice</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuqcpd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1kuq1y9</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>I don’t have nails. Ask questions — I’m from Colombia.</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o2vvzx7xpt2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1kuq0sh</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>I recently moved and was so scared to try a new salon but now I’m so happy!</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xy26l9ilpt2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1kupss1</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>What do u think of this?</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kupss1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1kups2v</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>I asked for 90s celestial whimsy goth and my nail tech understood the assignment</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/puupgh58nt2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1kupru4</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Square or Almond? (Re upload)</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kupru4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1kupq7z</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Getting certified</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kupq7z/getting_certified/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1kupi2l</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>is BIAB/Gel just as damaging as acrylic?</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kupi2l/is_biabgel_just_as_damaging_as_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1kup03i</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Any Good Fake Nail Sites?</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kup03i/any_good_fake_nail_sites/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1kuoyse</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>First time Chrome nails</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/no6k7mekft2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1kuowlj</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Design vs Completion :3</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuowlj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1kuofym</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>First time doing an structured gel mani on my self</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuofym</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1kuogcl</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>E File on shellac nails</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pc6g9x3xat2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1kuopqr</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Proud of my nail growth journey!</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/48tvk5j9dt2f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1kuomm0</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>First time trying out a cat eye mani</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuomm0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1kuohl7</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>First time trying out a cat eye mani</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuohl7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1kuoe7r</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Freshies</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nqafy2wdat2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1kunrpt</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Why does nothing stay on my nails?</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zwots6hq4t2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1kumhd4</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Help!!</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kumhd4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1kunq77</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>PSA</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kunq77/psa/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1kuo14o</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>Latina vibes vs Classic, How is better?</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuo14o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1kunz2y</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Was scrolling fron page and this sub came up, I want to share my GF last 2 Halloween sets</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kunz2y/was_scrolling_fron_page_and_this_sub_came_up_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1kunzga</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>I wanted to show off my lana del ray inspired nails🧍🏻‍♀️💕</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kunzga</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1kunxcu</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>First time doing this 😭</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/20sl6b4b6t2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1kunnso</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Best nails color/shape for my skin tone</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ozt2zaz3t2f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1kunn89</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>First time in decades I get acrylics. I’m 71 and my nails are no longer as strong as they were at one time</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ox9g9qu3t2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1kunlhb</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Coraline vibes?</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kunlhb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1kunh7t</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Goodnight moon 🌙 ✨</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kunh7t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1kungnn</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>One of my favourite sets I’ve ever had ✨</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/besdsua52t2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1kun74v</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>New summer claws!!</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kun74v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1kun5d5</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>I haven't gotten acrylics in ages, do these look too chunky? Is it because they're shorter?</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kun5d5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1kumx0u</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Square or almond?</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kumx0u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1kumlsi</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Similar nail colors?</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4tsiqxgvus2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1kumlqr</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Second Practice Set</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kumlqr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1kumjr9</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Such a gorgeous NAILS</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/08xlwzc9us2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1kume15</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Cowgirl up</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kume15</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1kum23k</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Haven't been to Salon in ages</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kum23k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1kum1hv</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Did them myself! How is it for my 2nd try at acrylics?</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eern82o5qs2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1kulx6k</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Neutral AF ☺️</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kulx6k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1kulqhc</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Got my nails done today! ^-^</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2kyj1xmons2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1kulpcl</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Curing question</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kulpcl/curing_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1kuloem</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Decided to have fun today - not sure what to think about it</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuloem</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1kullez</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>First time getting my nails done in years! Looking for ideas for next time :3</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j4lnswbjms2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1kulin5</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>7weeks Gel-X - no issues 🥰</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hk7cthxvls2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1kulcdt</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Finally got some sacred heart nails!</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/icrgzqsgks2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1kukp75</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>First time doing gel x and using blooming gel!</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kukp75</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1kul8xp</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Press On question</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pmybcuenjs2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1kul4qy</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Kids press ons on me</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m5pxkt2pis2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1kukyut</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Square Nails</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tsg9kgbchs2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1kukxaf</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Love these😻😻</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kukxaf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1kukt9r</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>So simple but fun.</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kukt9r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1kuklen</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Builder Gel Question</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kuklen/builder_gel_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1kuk9ru</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>❤️</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3tua0kolbs2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1kuk09t</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Frenchies</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuk09t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1kujkax</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Cat eye ✨and pink 🩷👣</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7nf0szpq5s2f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1kuj656</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>This is my second nail set done on myself. I bought a practice hand and did about 30 practice nails before doing this set. How’s it look?</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuj656</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1kuil0s</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Weird question about nail file types</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kuil0s/weird_question_about_nail_file_types/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1kuikf2</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Which Type of Manicure</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kuikf2/which_type_of_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1kuijwc</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Any good Memorial Day Sales this weekend in the U.S.?</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kuijwc/any_good_memorial_day_sales_this_weekend_in_the_us/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1kui79b</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Nail day!! 💙🌀</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kui79b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1kuidul</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Cut through natural nail while cutting off charm</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kuidul/cut_through_natural_nail_while_cutting_off_charm/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1kuhs7a</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Hema free gel polish recommendations</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1kuhs7a/hema_free_gel_polish_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1kuvcai</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Best place in Australia to get quick dry to coat? Eg.seche vite?</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kuvcai/best_place_in_australia_to_get_quick_dry_to_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1kuv31b</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Dupe suggestions DRUGSTORE ONLY</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yruhpjun6v2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1kuv191</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>How do you decide what colour to paint?</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuv191</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1kuuhhv</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>Rec requestw</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yqz1zfwuzu2f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1kuud66</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>ILNP - Deep Space</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tzystxejyu2f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1kuu813</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Shiny, sparkly light greens</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuu813</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1kutxgo</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Colors like Mooncat’s Poems for a Harvest Moon?</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ggacq7ptu2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1kutnb3</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Kathleen &amp; Co’s Linger</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kutnb3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1kutlhr</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>Go fish! 🪼🐟🪸</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kutlhr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1kusgkb</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer haul - including mystery protos and a GWP!</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kusgkb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1kus4um</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>Where to buy Seche Restore in Canada?</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kus4um/where_to_buy_seche_restore_in_canada/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1kus1rs</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>OPI eco for it</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kus1rs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1kurq41</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>My brain processed this in polish 😂</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pubuyca07n2f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1kurptx</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Cosmic Polish - Stormy Sunset</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rap51z7m6u2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1kurltu</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>actually loving this combo???</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wbk7vlgi5u2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1kurjab</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>Rogue Lacquer has THE BEST flakies!</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kurjab</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1kur8zm</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Mix n matched for a weekend at home</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kur8zm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1kur0ak</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>Help me find a shade like this - marigold / orange yellow</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/33urqdkhzt2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1kuqxx1</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>Mix up polish!</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m9uw7rssyt2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1kuqxuc</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>Blurple sparkle makes me :D</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuqxuc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1kuqqby</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>Swatch of Kings and Queens next to swatch of Blood Moon by Moon Cat?</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kuqqby/swatch_of_kings_and_queens_next_to_swatch_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1kuq027</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Three different By Dany Vianna flakies and some thoughts</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuq027</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1kupyql</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Psilocybin &amp; Panaeolus</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ejkxxmk1pt2f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1kupypu</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>Love This Pink</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kupypu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1kupw7h</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>Forbidden 🍏</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3sxqgv6cot2f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1kupozk</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>first time doing cat eye nails!</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kupozk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1kuph34</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>Fields of Elysium by Mooncat</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g8v9yjlakt2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1kup3pj</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>PFD Salamandra 🔥</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kup3pj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1kuoaw9</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>Help, I have been betrayed</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuoaw9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1kuo0qp</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>Emily de Molly order</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuo0qp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1kunjzj</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Stellar Evolution 🌟</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kunjzj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1kunit1</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>Will Liquid Latex in Bulk Dry Up?</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kunit1/will_liquid_latex_in_bulk_dry_up/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1kundp7</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>Base coat for toes?</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aof3w7fi1t2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1kud60e</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Painful, overfiled nails :(</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mgirh6ymrq2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1kukluh</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>When in doubt, put it over black and add a magnetic topper</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y6i2bf8des2f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1kuktoq</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Thank you!</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q9tkibs5gs2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1kumkb1</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>Slowly Going Through My BKL Stash</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kumkb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1kulyh0</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>Trying to achieve nails in second pic. I’m new to doing nails, and I can never achieve the flawless glass like finish in salon nails. Any tips?</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kulyh0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1kulqu7</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Looking for a dupe of a March HHC shade: All Mixed Up Lacquer Get OFF My Lawn!</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kulqu7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1kulfwo</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Even The Penguins Are Pissed🐧😠</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kulfwo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1kukooe</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>Cameo is pretty 😍</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d5u0dx21fs2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1kukh2u</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Why doesn’t my magnetic effect “lock” in?</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5yu3e44ads2f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1kukfp3</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Markartt Organizer Users - UV Protection</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kukfp3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1kujr0l</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>The perfect Spring shade</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kujr0l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1kujaqk</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Does PPU sell Cuticula QDTC?</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kujaqk/does_ppu_sell_cuticula_qdtc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1kuj57a</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>Bought a polish I don't care for, just for the meme 🙃</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c1s0pj0d2s2f1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1kuj2n6</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>The blue of my life 🤩</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuj2n6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1kui69g</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>Memorial Day Weekend sales thread</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kui69g/memorial_day_weekend_sales_thread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1kuhxuo</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>‘50’ is flirty, sparkly, and magnetic. Literally.</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuhxuo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1kuhwli</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>Like a streak of lightning across the night sky ⚡</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/b47uq1ajsr2f1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1kuhvbf</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>Cursed mani unlocked: Swollen Finger Neutral</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuhvbf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1kuhq3r</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>Newish brand, Prism Parade. Love the polish, brush is hot garbage. Thoughts?</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuhq3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1kuhgc8</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>🐙👁️👍 Squid Eye Thumb. brought to you courtesy of last nights edible 🌱💖🫠</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuhgc8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1kuh8km</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>Lateral naild folds are JANKY</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuh8km</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1kuge2z</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>Sometimes only a red will do</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuge2z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1kug4u2</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>I like to call this combo "They Will Never Find You Quite Literally Dead Inside"</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kug4u2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1kufrs6</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>First time using builder gel 🥴</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kufrs6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1kufg2e</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>Brown marks on nails</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7bsmicyl9r2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1kufdob</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>ILNP Sugar Cube</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pgq71j04zp2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1kuf2bd</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>Who does a flakie as gorgeous as Mooncat Maelstrom?</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1kuf2bd/who_does_a_flakie_as_gorgeous_as_mooncat_maelstrom/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1kuezzr</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>i graduated! while wearing my favorite polish.</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuezzr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1kuel1a</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>Tie-dye nails matching the dress!</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuel1a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1kuehy6</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>Reflection Pool with Flair</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hf8haz292r2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1kuehbv</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>Cadillacquer - Nightbook</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuehbv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1kudd1u</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>❤️Keith Haring❤️</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kudd1u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1kucw7i</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>Should we maybe just… cook him? 🥰</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6rni2k9hpq2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1kub9ta</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>long time lurker, first time poster, big glitter fan</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kub9ta</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1kucksf</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>Anyone know how to help this stop happening?</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ajatsfutmq2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1kuc9rt</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>Blue Bird Lacquer Turn it Up to Eleven</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuc9rt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1kuc53x</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>Algae Nail and Ketchup and Mustard Nails</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuc53x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1kuawjj</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>After the rain</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/38jpfpak8q2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1kuastm</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>Cracked browns?</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b80oe6zi7q2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1kuar6r</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>I love it and I hate it at the same time</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuar6r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1kua0oc</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>Zoya - Freja</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kua0oc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1ku77hu</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>My favorit way of magnitizing ATM</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ku77hu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1ku6qyf</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>The most insane teal I’ve ever seen🩵</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ku6qyf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1kutm48</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>Fairy core 🧚🏾‍♀️</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kutm48</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1kusw3o</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>My most recent nails 💛🐝</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kusw3o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1kum81x</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>Summer set! Love them 💚</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kum81x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1kum66n</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>Grunge cat eye nailssss</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kum66n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1kulnmy</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>Long pink birthday set</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kulnmy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1kui8zb</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>First time doing nail art</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kui8zb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1kui2a6</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>Need your help to create a master list of nail theme ideas (you can go as weird and niche as you want)</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kui2a6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1kui1fk</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>🩷🩷new nail</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mt0759tktr2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1kui039</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>Nailart from Japan 🥹</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kui039</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1kuhlm6</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>Misty winter forests in summer!</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kuhlm6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1kuhalv</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>Inspired by all the spring butterfly nails</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yjcwejztnr2f1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1kugu9s</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>A post for the Long Nail lovers! Fun with Cat Eye</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kugu9s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1kucshi</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>New set finally done💙</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1kucshi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1kuaa29</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>Where/who do you buy nail stickers from?</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1kuaa29/wherewho_do_you_buy_nail_stickers_from/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>